<commit_message>
Added HR Create Account
</commit_message>
<xml_diff>
--- a/Schema/Schema.xlsx
+++ b/Schema/Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EasyWeb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Easy Web\Truventa\Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608B72C1-D54F-4B91-9673-960076E8F918}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848375E4-E4B8-47CA-A3B6-E1A7EB06B5AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="569" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="569" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final " sheetId="2" r:id="rId1"/>
@@ -494,9 +494,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -531,6 +528,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -873,60 +873,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
       <c r="N1" s="7"/>
-      <c r="O1" s="32" t="s">
+      <c r="O1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -945,7 +945,7 @@
         <v>69</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -970,10 +970,10 @@
       <c r="O3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="23" t="s">
+      <c r="P3" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="Q3" s="30" t="s">
         <v>55</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -985,13 +985,13 @@
       <c r="T3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="23" t="s">
+      <c r="U3" s="22" t="s">
         <v>59</v>
       </c>
       <c r="V3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="W3" s="25" t="s">
+      <c r="W3" s="24" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="23">
+      <c r="G4" s="22">
         <v>32</v>
       </c>
       <c r="H4" s="3">
@@ -1027,14 +1027,14 @@
       </c>
       <c r="N4" s="7"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="31"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="30"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="24"/>
+      <c r="U4" s="23"/>
       <c r="V4" s="3"/>
-      <c r="W4" s="25">
+      <c r="W4" s="24">
         <v>18</v>
       </c>
     </row>
@@ -1047,7 +1047,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="23"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -1056,14 +1056,14 @@
       <c r="M5" s="3"/>
       <c r="N5" s="7"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="31"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="30"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
-      <c r="U5" s="24"/>
+      <c r="U5" s="23"/>
       <c r="V5" s="3"/>
-      <c r="W5" s="26"/>
+      <c r="W5" s="25"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1074,7 +1074,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="23"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -1083,64 +1083,64 @@
       <c r="M6" s="3"/>
       <c r="N6" s="7"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="31"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="30"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
-      <c r="U6" s="24"/>
+      <c r="U6" s="23"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="26"/>
+      <c r="W6" s="25"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="K10" s="34" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="K10" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="22" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1178,16 +1178,16 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="29">
         <v>123</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="27">
         <v>44227</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="22">
         <v>32</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <v>21</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1219,16 +1219,16 @@
       <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" s="30">
+      <c r="A14" s="29">
         <v>124</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="27">
         <v>44227</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="22">
         <v>32</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="22">
         <v>21</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1250,16 +1250,16 @@
       <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="30">
+      <c r="A15" s="29">
         <v>125</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="27">
         <v>44227</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="22">
         <v>32</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="22">
         <v>21</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1281,10 +1281,10 @@
       <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
@@ -1331,32 +1331,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="G1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
       <c r="N1" s="7"/>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
       <c r="V1" s="6"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -1527,15 +1527,15 @@
       <c r="U6" s="3"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
       <c r="I10" s="16"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
@@ -1731,15 +1731,15 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="H19" s="22" t="s">
+      <c r="H19" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G21" s="9"/>

</xml_diff>

<commit_message>
Login and MR finalized
</commit_message>
<xml_diff>
--- a/Schema/Schema.xlsx
+++ b/Schema/Schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Easy Web\Truventa\Schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Truventa\Schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848375E4-E4B8-47CA-A3B6-E1A7EB06B5AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4100AD2A-7AD4-4E0D-9A2F-465F105ED936}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="569" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
   <si>
     <t>MR</t>
   </si>
@@ -245,6 +236,15 @@
   </si>
   <si>
     <t>pin</t>
+  </si>
+  <si>
+    <t>SickLeaves</t>
+  </si>
+  <si>
+    <t>CasualLeaves</t>
+  </si>
+  <si>
+    <t>UnpaidLeaves</t>
   </si>
 </sst>
 </file>
@@ -849,7 +849,7 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,13 +958,13 @@
         <v>7</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="3" t="s">

</xml_diff>